<commit_message>
Final Assessment 2: Task 2
1. Introduced the concept of abstraction in class snake, gameboard and prey
2. Added public methods conforming to the user stories
3. Updated the product backlog according to the progress of week 9
</commit_message>
<xml_diff>
--- a/snakegame_v1/Product Backlog.xlsx
+++ b/snakegame_v1/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scuonline-my.sharepoint.com/personal/p_pundir_10_student_scu_edu_au/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhubneshwarchandel/Desktop/Github/snakegame_v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{5A72AAD7-ABD2-3C4B-96AB-FFB782214E29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4841D712-BE30-BC43-AF0C-BBAC1C1DB569}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76AB04C-529B-BA4D-84CE-23115B51B53D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{49C32462-D2B8-4175-AE19-832EFB3F644D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{49C32462-D2B8-4175-AE19-832EFB3F644D}"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>Week 9</t>
   </si>
@@ -151,9 +151,6 @@
     <t xml:space="preserve">the gameboard window to close </t>
   </si>
   <si>
-    <t>the gameboard to be visible on the screen</t>
-  </si>
-  <si>
     <t>the game board to be of black color</t>
   </si>
   <si>
@@ -221,6 +218,12 @@
   </si>
   <si>
     <t>the game to be over if the snake touches border</t>
+  </si>
+  <si>
+    <t>Snake Logic</t>
+  </si>
+  <si>
+    <t>Gameboard Logic</t>
   </si>
 </sst>
 </file>
@@ -383,12 +386,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +393,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F2A6E6-5A3B-4CAD-BC9F-023E52339F74}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -730,40 +733,40 @@
       <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="35"/>
+      <c r="B4" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="40"/>
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -807,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -815,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -831,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -839,21 +842,21 @@
         <v>6</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="8">
+      <c r="C15" s="8"/>
+      <c r="D15" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="8">
         <v>7</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="8"/>
-      <c r="D16" s="36" t="s">
-        <v>39</v>
+      <c r="D16" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -861,7 +864,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -869,7 +872,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -877,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -885,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -893,33 +896,25 @@
         <v>12</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="8">
+      <c r="C22" s="8"/>
+      <c r="D22" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="8">
         <v>13</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="8"/>
-      <c r="D23" s="36" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="8">
-        <v>14</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="18"/>
+      <c r="D24" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -934,10 +929,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDA2708-75B5-4180-9C4B-08F40A18D95A}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,7 +980,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -1143,7 +1138,7 @@
       <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="35">
         <v>1</v>
       </c>
       <c r="G13" s="6"/>
@@ -1209,9 +1204,9 @@
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="37">
+        <v>59</v>
+      </c>
+      <c r="F19" s="35">
         <v>1</v>
       </c>
       <c r="G19" s="6"/>
@@ -1223,10 +1218,10 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="37"/>
+      <c r="D20" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="35"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1238,10 +1233,10 @@
         <v>31</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="37">
         <v>0.2</v>
       </c>
       <c r="H21" s="6"/>
@@ -1254,7 +1249,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1265,72 +1260,72 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="D24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="40">
+      <c r="G25" s="38">
         <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="D26" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="D27" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="D28" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="40">
+      <c r="G29" s="38">
         <v>0.2</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="D30" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
-      <c r="D31" s="36"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
-      <c r="D32" s="36"/>
+      <c r="D32" s="34"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
-      <c r="D33" s="36"/>
+      <c r="D33" s="34"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
@@ -1347,24 +1342,52 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="37">
+      <c r="A36" s="9"/>
+      <c r="B36" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="9">
+      <c r="A37" s="9"/>
+      <c r="B37" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
         <v>5</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E40" s="8">
         <v>4</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F40" s="14">
         <v>0</v>
       </c>
     </row>

</xml_diff>